<commit_message>
[Soubarnika]Refactored:Added screenshots and KeyActions
</commit_message>
<xml_diff>
--- a/LinkedInTesting_Selenium/TestDataFiles/Signup_TestData.xlsx
+++ b/LinkedInTesting_Selenium/TestDataFiles/Signup_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soubarnika.v\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soubarnika.v\source\repos\LinkedInTesting_Selenium\LinkedInTesting_Selenium\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t>venkatsoumuthu@gmail.com</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>venkatsou</t>
+  </si>
+  <si>
+    <t>muthu</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
   </si>
 </sst>
 </file>
@@ -361,30 +376,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>9629522931</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>9629459258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>